<commit_message>
delete images, modify e4 tableau, add carrousel
</commit_message>
<xml_diff>
--- a/fichiers/tableauSyntheseE4.xlsx
+++ b/fichiers/tableauSyntheseE4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Stage\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\portfolio\fichiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A58C32-DD5F-4714-A0E4-075388B4FAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358BB7DA-AAE1-4FA9-824F-92B5ABCA3FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -211,6 +211,24 @@
   </si>
   <si>
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
+  </si>
+  <si>
+    <t>modifier le site web de l'association</t>
+  </si>
+  <si>
+    <t>02/12/2024 - 26/01/2025</t>
+  </si>
+  <si>
+    <t>faire l'intranet du site</t>
+  </si>
+  <si>
+    <t>formation wordpress</t>
+  </si>
+  <si>
+    <t>02/12/2024 - 10/12/2024</t>
+  </si>
+  <si>
+    <t>11/12/2024 - ?</t>
   </si>
 </sst>
 </file>
@@ -731,12 +749,45 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,39 +811,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1105,8 +1123,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1119,83 +1137,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="29"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="38" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="38"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="42" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="47"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="47" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -1218,8 +1236,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="16" t="s">
         <v>18</v>
       </c>
@@ -1275,16 +1293,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="43"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1844,16 +1862,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2252,16 +2270,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="46"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2299,13 +2317,27 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="A28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="H28" s="8"/>
       <c r="I28"/>
       <c r="J28"/>
@@ -2344,12 +2376,20 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
       <c r="I29"/>
@@ -2389,14 +2429,22 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2843,17 +2891,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
change project stage index
</commit_message>
<xml_diff>
--- a/fichiers/tableauSyntheseE4.xlsx
+++ b/fichiers/tableauSyntheseE4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\portfolio\fichiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358BB7DA-AAE1-4FA9-824F-92B5ABCA3FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189306AF-DBCC-44AA-80CE-9429339FE1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -135,42 +135,15 @@
 </t>
   </si>
   <si>
-    <t>freecodecamp html/css</t>
-  </si>
-  <si>
-    <t>04/09/2023 au 18/09/23</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>pix</t>
-  </si>
-  <si>
-    <t>9/11/23 au 14/11/23</t>
-  </si>
-  <si>
-    <t>site github - paniers gourmands</t>
-  </si>
-  <si>
     <t>25/09/23 au 09/10/23</t>
   </si>
   <si>
-    <t>certification packet tracer</t>
-  </si>
-  <si>
-    <t>25/09/23 au 27/10/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">création d'un site web accessible </t>
-  </si>
-  <si>
     <t>09/01/24 au 27/02/24</t>
   </si>
   <si>
-    <t>création s'un site MVC avec CRUD en PHP</t>
-  </si>
-  <si>
     <t>05/03/24 au 23/04/24</t>
   </si>
   <si>
@@ -183,15 +156,9 @@
     <t>Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
-    <t>faire de la maintenance informatique</t>
-  </si>
-  <si>
     <t>13/05/24 au 21/05/24</t>
   </si>
   <si>
-    <t>création de script avec macro VBA (Excel)</t>
-  </si>
-  <si>
     <t>14/05/24 à 05/07/2024</t>
   </si>
   <si>
@@ -201,27 +168,15 @@
     <t>22/05/24 à 05/07/2024</t>
   </si>
   <si>
-    <t>installation et sécurisation des postes informatiques</t>
-  </si>
-  <si>
     <t>17/05/24 au 21/05/24</t>
   </si>
   <si>
-    <t>présentation d'une application Hairnet pour les professeurs d'esthétiques, coiffure</t>
-  </si>
-  <si>
     <t>Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t>modifier le site web de l'association</t>
-  </si>
-  <si>
     <t>02/12/2024 - 26/01/2025</t>
   </si>
   <si>
-    <t>faire l'intranet du site</t>
-  </si>
-  <si>
     <t>formation wordpress</t>
   </si>
   <si>
@@ -229,6 +184,39 @@
   </si>
   <si>
     <t>11/12/2024 - ?</t>
+  </si>
+  <si>
+    <t>projet création de site web : Les Paniers Gourmands</t>
+  </si>
+  <si>
+    <t>création d'un site web accessible (projet AP) : paysASE</t>
+  </si>
+  <si>
+    <t>création s'un site MVC avec CRUD en PHP : Restotop</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x </t>
+  </si>
+  <si>
+    <t>faire de la maintenance informatique (rangement des équipements)</t>
+  </si>
+  <si>
+    <t>création de script avec macro VBA (Excel) : création de planning pour les examens</t>
+  </si>
+  <si>
+    <t>installation et sécurisation des postes informatiques (installation et activation d'antivirus)</t>
+  </si>
+  <si>
+    <t>présentation d'une application Hairnet pour les professeurs d'esthétiques et de coiffure</t>
+  </si>
+  <si>
+    <t>modifier le site web de l'association (design, ajout de contenu, ajout d'extensions,...)</t>
+  </si>
+  <si>
+    <t>faire l'intranet du site : ajout d'un calendrier interractif, création de compte pour les membres,…)</t>
   </si>
 </sst>
 </file>
@@ -770,9 +758,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -784,33 +799,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1123,70 +1111,70 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="18.54296875" style="1" customWidth="1"/>
-    <col min="9" max="43" width="10.81640625" customWidth="1"/>
-    <col min="44" max="16384" width="10.81640625" style="1"/>
+    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="18.5546875" style="1" customWidth="1"/>
+    <col min="9" max="43" width="10.77734375" customWidth="1"/>
+    <col min="44" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="35"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+    </row>
+    <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="36" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="29" t="s">
         <v>6</v>
       </c>
@@ -1197,7 +1185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>9</v>
       </c>
@@ -1210,10 +1198,10 @@
       <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -1235,9 +1223,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="48"/>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="16" t="s">
         <v>18</v>
       </c>
@@ -1292,17 +1280,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1339,22 +1327,26 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="49.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="E9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
-        <v>27</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="21"/>
       <c r="H9" s="22"/>
       <c r="I9"/>
       <c r="J9"/>
@@ -1392,20 +1384,26 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="21"/>
+        <v>43</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="H10" s="22" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1443,27 +1441,27 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>31</v>
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>27</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
+        <v>25</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1500,23 +1498,29 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
+        <v>25</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1553,27 +1557,15 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>27</v>
-      </c>
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
-      <c r="F13" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1610,27 +1602,15 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>27</v>
-      </c>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1667,29 +1647,15 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>27</v>
-      </c>
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1726,7 +1692,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
@@ -1771,7 +1737,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
@@ -1816,7 +1782,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
@@ -1861,17 +1827,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1908,22 +1874,22 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
@@ -1963,24 +1929,24 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2018,23 +1984,23 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22"/>
@@ -2073,23 +2039,23 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23"/>
@@ -2128,9 +2094,9 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B24" s="25">
         <v>45475</v>
@@ -2140,7 +2106,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24"/>
@@ -2179,7 +2145,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
@@ -2224,7 +2190,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -2269,17 +2235,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="46"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2316,27 +2282,27 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28"/>
@@ -2375,20 +2341,20 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
@@ -2428,22 +2394,22 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -2481,7 +2447,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="11"/>
       <c r="C31" s="7"/>
@@ -2526,7 +2492,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="11"/>
       <c r="C32" s="7"/>
@@ -2571,7 +2537,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="11"/>
       <c r="C33" s="7"/>
@@ -2616,7 +2582,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="11"/>
       <c r="C34" s="7"/>
@@ -2661,7 +2627,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="12"/>
       <c r="C35" s="9"/>
@@ -2706,7 +2672,7 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="13"/>
       <c r="C36" s="3"/>
@@ -2891,17 +2857,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
add new projects and modify contact form
</commit_message>
<xml_diff>
--- a/fichiers/tableauSyntheseE4.xlsx
+++ b/fichiers/tableauSyntheseE4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\portfolio\fichiers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189306AF-DBCC-44AA-80CE-9429339FE1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A969C5F-1D58-44D5-9532-D31029C5DC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>faire l'intranet du site : ajout d'un calendrier interractif, création de compte pour les membres,…)</t>
+  </si>
+  <si>
+    <t>créer les biletteries pour l'association et le rajouter sur le site web</t>
+  </si>
+  <si>
+    <t>02/12/24 - 11/01/25</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -296,10 +302,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="16"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
     </font>
@@ -654,7 +656,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -716,16 +718,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -758,12 +757,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -787,18 +798,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1111,8 +1110,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1125,107 +1124,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="36"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="45" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="29" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="33"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="16" t="s">
         <v>18</v>
       </c>
@@ -1281,16 +1280,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="42"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1328,26 +1327,26 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="49.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="F9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1391,18 +1390,18 @@
       <c r="B10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="C10" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>46</v>
       </c>
       <c r="I10"/>
@@ -1448,18 +1447,18 @@
       <c r="B11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="22" t="s">
+      <c r="C11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="21" t="s">
         <v>25</v>
       </c>
       <c r="I11"/>
@@ -1505,20 +1504,20 @@
       <c r="B12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="22" t="s">
+      <c r="C12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="21" t="s">
         <v>25</v>
       </c>
       <c r="I12"/>
@@ -1560,12 +1559,12 @@
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1605,12 +1604,12 @@
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1650,12 +1649,12 @@
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1828,16 +1827,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2098,7 +2097,7 @@
       <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="24">
         <v>45475</v>
       </c>
       <c r="C24" s="7"/>
@@ -2236,16 +2235,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="45"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2448,13 +2447,21 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="G31" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H31" s="8"/>
       <c r="I31"/>
       <c r="J31"/>
@@ -2857,17 +2864,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>